<commit_message>
fix bug of heatmap paramter
</commit_message>
<xml_diff>
--- a/tests/out.group.info.xlsx
+++ b/tests/out.group.info.xlsx
@@ -1,385 +1,396 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiyuting/Documents/projects/ball/package/gvmap/tests/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17520" windowHeight="12000" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="heatmap_1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="heatmap_2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="heatmap_3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="sample_list" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="heatmap_1" sheetId="1" r:id="rId1"/>
+    <sheet name="heatmap_2" sheetId="2" r:id="rId2"/>
+    <sheet name="heatmap_3" sheetId="3" r:id="rId3"/>
+    <sheet name="sample_list" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
-  <si>
-    <t xml:space="preserve">row_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PFKP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENDOD1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCAT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1orf186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLC45A3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLA-DMB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLA-DPB1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLA-DRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPR3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIITA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTPRCAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FADS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGFL7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLA-DRB1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLA-DPA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIST1H2BM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIST1H2BL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIST1H2BH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSPA1B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANXA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBG2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTD-2328D6.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT-RNR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT-RNR2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALOX12P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLC40A1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FBN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EIF4E3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MX1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMPK2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFI44L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFI6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNORD116-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EREG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNORA74B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNORA53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNORA74A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCARNA5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFA4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTSG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BPI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIN7A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OLFM4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SYNE2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PGLYRP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NFAM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP5B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MYO7B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NKG7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STOX2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CST7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARHGAP24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HK3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLPI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYSTM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STX11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD24P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S100A9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S100A8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OLR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COL17A1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LYZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANXA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEACAM8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPP7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABCA13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UGCG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FCAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEACAM6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TACSTD2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LRG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARCKS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S100P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RGL4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PADI2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MNDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SORT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THBS4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPCEF1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NFIL3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHD7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PFKFB3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1001</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="119">
+  <si>
+    <t>row_name</t>
+  </si>
+  <si>
+    <t>gap</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>PFKP</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>FLT3</t>
+  </si>
+  <si>
+    <t>ENDOD1</t>
+  </si>
+  <si>
+    <t>BCAT1</t>
+  </si>
+  <si>
+    <t>C1orf186</t>
+  </si>
+  <si>
+    <t>SLC45A3</t>
+  </si>
+  <si>
+    <t>HLA-DMB</t>
+  </si>
+  <si>
+    <t>HLA-DPB1</t>
+  </si>
+  <si>
+    <t>HLA-DRA</t>
+  </si>
+  <si>
+    <t>NPR3</t>
+  </si>
+  <si>
+    <t>CD74</t>
+  </si>
+  <si>
+    <t>CIITA</t>
+  </si>
+  <si>
+    <t>CD34</t>
+  </si>
+  <si>
+    <t>PTPRCAP</t>
+  </si>
+  <si>
+    <t>FADS2</t>
+  </si>
+  <si>
+    <t>EGFL7</t>
+  </si>
+  <si>
+    <t>TRH</t>
+  </si>
+  <si>
+    <t>GBP4</t>
+  </si>
+  <si>
+    <t>HLA-DRB1</t>
+  </si>
+  <si>
+    <t>KIT</t>
+  </si>
+  <si>
+    <t>HLA-DPA1</t>
+  </si>
+  <si>
+    <t>PROM1</t>
+  </si>
+  <si>
+    <t>HIST1H2BM</t>
+  </si>
+  <si>
+    <t>HIST1H2BL</t>
+  </si>
+  <si>
+    <t>HIST1H2BH</t>
+  </si>
+  <si>
+    <t>CD52</t>
+  </si>
+  <si>
+    <t>LDLR</t>
+  </si>
+  <si>
+    <t>HSPA1B</t>
+  </si>
+  <si>
+    <t>EMP1</t>
+  </si>
+  <si>
+    <t>ANXA2</t>
+  </si>
+  <si>
+    <t>HBA2</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>HBA1</t>
+  </si>
+  <si>
+    <t>HBB</t>
+  </si>
+  <si>
+    <t>HBG2</t>
+  </si>
+  <si>
+    <t>CTD-2328D6.1</t>
+  </si>
+  <si>
+    <t>MT-RNR1</t>
+  </si>
+  <si>
+    <t>MT-RNR2</t>
+  </si>
+  <si>
+    <t>TTN</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>ALOX12P2</t>
+  </si>
+  <si>
+    <t>SLC40A1</t>
+  </si>
+  <si>
+    <t>FBN1</t>
+  </si>
+  <si>
+    <t>EIF4E3</t>
+  </si>
+  <si>
+    <t>MX1</t>
+  </si>
+  <si>
+    <t>CMPK2</t>
+  </si>
+  <si>
+    <t>IFI44L</t>
+  </si>
+  <si>
+    <t>IFI6</t>
+  </si>
+  <si>
+    <t>SNORD116-20</t>
+  </si>
+  <si>
+    <t>EREG</t>
+  </si>
+  <si>
+    <t>SNORA74B</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>SNORA53</t>
+  </si>
+  <si>
+    <t>SNORA74A</t>
+  </si>
+  <si>
+    <t>SCARNA5</t>
+  </si>
+  <si>
+    <t>DEFA4</t>
+  </si>
+  <si>
+    <t>DEFA3</t>
+  </si>
+  <si>
+    <t>CTSG</t>
+  </si>
+  <si>
+    <t>BPI</t>
+  </si>
+  <si>
+    <t>LIN7A</t>
+  </si>
+  <si>
+    <t>OLFM4</t>
+  </si>
+  <si>
+    <t>SYNE2</t>
+  </si>
+  <si>
+    <t>PGLYRP1</t>
+  </si>
+  <si>
+    <t>NFAM1</t>
+  </si>
+  <si>
+    <t>AP5B1</t>
+  </si>
+  <si>
+    <t>MYO7B</t>
+  </si>
+  <si>
+    <t>NKG7</t>
+  </si>
+  <si>
+    <t>STOX2</t>
+  </si>
+  <si>
+    <t>CST7</t>
+  </si>
+  <si>
+    <t>ARHGAP24</t>
+  </si>
+  <si>
+    <t>HK3</t>
+  </si>
+  <si>
+    <t>SLPI</t>
+  </si>
+  <si>
+    <t>TCN1</t>
+  </si>
+  <si>
+    <t>CYSTM1</t>
+  </si>
+  <si>
+    <t>STX11</t>
+  </si>
+  <si>
+    <t>CD24P4</t>
+  </si>
+  <si>
+    <t>S100A9</t>
+  </si>
+  <si>
+    <t>S100A8</t>
+  </si>
+  <si>
+    <t>OLR1</t>
+  </si>
+  <si>
+    <t>COL17A1</t>
+  </si>
+  <si>
+    <t>JAG1</t>
+  </si>
+  <si>
+    <t>LYZ</t>
+  </si>
+  <si>
+    <t>ARG1</t>
+  </si>
+  <si>
+    <t>ANXA3</t>
+  </si>
+  <si>
+    <t>CEACAM8</t>
+  </si>
+  <si>
+    <t>MPP7</t>
+  </si>
+  <si>
+    <t>ABCA13</t>
+  </si>
+  <si>
+    <t>UGCG</t>
+  </si>
+  <si>
+    <t>FCAR</t>
+  </si>
+  <si>
+    <t>CEACAM6</t>
+  </si>
+  <si>
+    <t>TACSTD2</t>
+  </si>
+  <si>
+    <t>LRG1</t>
+  </si>
+  <si>
+    <t>MARCKS</t>
+  </si>
+  <si>
+    <t>S100P</t>
+  </si>
+  <si>
+    <t>RGL4</t>
+  </si>
+  <si>
+    <t>PADI2</t>
+  </si>
+  <si>
+    <t>MNDA</t>
+  </si>
+  <si>
+    <t>SORT1</t>
+  </si>
+  <si>
+    <t>THBS4</t>
+  </si>
+  <si>
+    <t>IPCEF1</t>
+  </si>
+  <si>
+    <t>NFIL3</t>
+  </si>
+  <si>
+    <t>CHD7</t>
+  </si>
+  <si>
+    <t>PFKFB3</t>
+  </si>
+  <si>
+    <t>g0</t>
+  </si>
+  <si>
+    <t>col_name</t>
+  </si>
+  <si>
+    <t>M4003</t>
+  </si>
+  <si>
+    <t>M4004</t>
+  </si>
+  <si>
+    <t>M4001</t>
+  </si>
+  <si>
+    <t>M4002</t>
+  </si>
+  <si>
+    <t>M4005</t>
+  </si>
+  <si>
+    <t>M1002</t>
+  </si>
+  <si>
+    <t>M1003</t>
+  </si>
+  <si>
+    <t>M1005</t>
+  </si>
+  <si>
+    <t>M1004</t>
+  </si>
+  <si>
+    <t>M1001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -415,6 +426,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -696,14 +713,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -725,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -736,7 +753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -747,7 +764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -758,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -769,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -780,7 +797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -791,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -802,7 +819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -813,7 +830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -824,7 +841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -835,7 +852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -846,7 +863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -857,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -868,7 +885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -879,7 +896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -890,7 +907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -901,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -912,7 +929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -923,7 +940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -934,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -945,7 +962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -956,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -967,7 +984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -978,7 +995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -989,7 +1006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1000,7 +1017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1011,7 +1028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1022,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1033,7 +1050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1044,7 +1061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1055,7 +1072,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1066,7 +1083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1077,7 +1094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1088,7 +1105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1099,7 +1116,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1110,7 +1127,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1121,7 +1138,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1132,7 +1149,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1143,7 +1160,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1154,7 +1171,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1165,7 +1182,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1176,7 +1193,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1187,7 +1204,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1198,7 +1215,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1209,7 +1226,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1220,7 +1237,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1231,7 +1248,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1242,7 +1259,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1253,7 +1270,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1264,7 +1281,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -1275,7 +1292,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -1286,7 +1303,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -1297,7 +1314,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -1308,7 +1325,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -1319,7 +1336,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -1330,7 +1347,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -1341,7 +1358,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -1352,7 +1369,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -1363,7 +1380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -1374,7 +1391,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -1385,7 +1402,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -1396,7 +1413,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -1407,7 +1424,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -1418,7 +1435,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -1429,7 +1446,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -1440,7 +1457,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -1451,7 +1468,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -1462,7 +1479,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -1473,7 +1490,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -1484,7 +1501,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -1495,7 +1512,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -1506,7 +1523,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -1517,7 +1534,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -1528,7 +1545,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -1539,7 +1556,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -1550,7 +1567,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -1561,7 +1578,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -1572,7 +1589,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -1583,7 +1600,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -1594,7 +1611,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -1605,7 +1622,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -1616,7 +1633,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -1627,7 +1644,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -1638,7 +1655,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -1649,7 +1666,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -1660,7 +1677,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -1671,7 +1688,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -1682,7 +1699,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -1693,7 +1710,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -1704,7 +1721,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>97</v>
       </c>
@@ -1715,7 +1732,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -1726,7 +1743,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -1737,7 +1754,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>100</v>
       </c>
@@ -1748,7 +1765,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -1759,7 +1776,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -1770,7 +1787,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -1781,7 +1798,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>104</v>
       </c>
@@ -1792,7 +1809,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>105</v>
       </c>
@@ -1803,7 +1820,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>106</v>
       </c>
@@ -1816,24 +1833,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="3.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1855,7 +1872,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1866,7 +1883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1877,7 +1894,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1888,7 +1905,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1899,7 +1916,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1910,7 +1927,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1921,7 +1938,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1932,7 +1949,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1943,7 +1960,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1954,7 +1971,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1965,7 +1982,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1976,7 +1993,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1987,7 +2004,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1998,7 +2015,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2009,7 +2026,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2020,7 +2037,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -2031,7 +2048,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -2042,7 +2059,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2053,7 +2070,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -2064,7 +2081,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -2075,7 +2092,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -2086,7 +2103,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2097,7 +2114,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -2108,7 +2125,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -2119,7 +2136,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2130,7 +2147,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2141,7 +2158,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2152,7 +2169,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2163,7 +2180,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -2174,7 +2191,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -2187,24 +2204,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="3.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +2232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -2226,7 +2243,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -2237,7 +2254,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -2248,7 +2265,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -2259,7 +2276,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -2270,7 +2287,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -2281,7 +2298,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -2292,7 +2309,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -2303,7 +2320,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -2314,7 +2331,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -2325,7 +2342,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2336,7 +2353,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2347,7 +2364,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2358,7 +2375,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2369,7 +2386,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2380,7 +2397,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -2391,7 +2408,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2402,7 +2419,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2413,7 +2430,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2424,7 +2441,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2435,7 +2452,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2448,19 +2465,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -2471,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -2482,7 +2501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -2493,7 +2512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -2504,7 +2523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -2515,7 +2534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2526,7 +2545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -2537,7 +2556,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -2548,7 +2567,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -2559,7 +2578,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -2570,7 +2589,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -2583,6 +2602,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>